<commit_message>
Revert "Revert "Merge pull request #5 from dandz12/Ha's-branch""
This reverts commit 9b01ece93a4c787b3d0d3d6b80cd6086ba08118c.
</commit_message>
<xml_diff>
--- a/Dwayne & Ha & Danial Decision Matrix.xlsx
+++ b/Dwayne & Ha & Danial Decision Matrix.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ha Tran\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BumBum/Documents/ECE411-Practicum-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7090"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21280" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Project Proposal</t>
   </si>
@@ -50,9 +56,6 @@
     <t>Ha</t>
   </si>
   <si>
-    <t>Than</t>
-  </si>
-  <si>
     <t>Complexity</t>
   </si>
   <si>
@@ -120,12 +123,24 @@
   </si>
   <si>
     <t>Alarm</t>
+  </si>
+  <si>
+    <t>Useless Lock Box</t>
+  </si>
+  <si>
+    <t>Number Pad Buttons</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Thanh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -174,22 +189,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -197,7 +212,7 @@
       <left/>
       <right/>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -205,35 +220,35 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -241,44 +256,44 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -287,12 +302,12 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -300,18 +315,18 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -319,10 +334,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -330,7 +345,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -339,21 +354,21 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -363,7 +378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -399,21 +414,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -423,6 +423,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -468,15 +480,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -486,8 +489,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -807,75 +813,75 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A8" sqref="A8:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.453125" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" customWidth="1"/>
-    <col min="3" max="3" width="1.81640625" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" customWidth="1"/>
-    <col min="6" max="6" width="1.81640625" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" customWidth="1"/>
-    <col min="8" max="8" width="16.54296875" customWidth="1"/>
-    <col min="9" max="9" width="16.1796875" customWidth="1"/>
-    <col min="10" max="10" width="12.54296875" customWidth="1"/>
-    <col min="11" max="11" width="9.1796875" customWidth="1"/>
-    <col min="12" max="12" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="1.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="1.83203125" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" customWidth="1"/>
+    <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" customWidth="1"/>
+    <col min="10" max="10" width="12.5" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="40"/>
+      <c r="H1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>13</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>14</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="10">
         <v>3</v>
@@ -884,31 +890,31 @@
         <v>1</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="10">
         <v>3</v>
       </c>
-      <c r="I2" s="32">
-        <v>3</v>
-      </c>
-      <c r="J2" s="29">
-        <v>3</v>
-      </c>
-      <c r="K2" s="20">
+      <c r="I2" s="31">
+        <v>3</v>
+      </c>
+      <c r="J2" s="28">
+        <v>3</v>
+      </c>
+      <c r="K2" s="15">
         <v>1</v>
       </c>
-      <c r="L2" s="20">
-        <v>2</v>
-      </c>
-      <c r="M2" s="20">
+      <c r="L2" s="15">
+        <v>2</v>
+      </c>
+      <c r="M2" s="15">
         <f>-SUM(E2:E4)*$E$15-SUM(H2:H4)*$H$15+I2*$I$15+J2*$J$15+K2*$K$15+L2*$L$15</f>
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="17"/>
-      <c r="B3" s="24"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="20"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="8">
         <v>2</v>
       </c>
@@ -918,20 +924,20 @@
         <v>2</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" s="11">
         <v>2</v>
       </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-    </row>
-    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="18"/>
-      <c r="B4" s="25"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+    </row>
+    <row r="4" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="2">
         <v>3</v>
       </c>
@@ -942,24 +948,24 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="13"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-    </row>
-    <row r="5" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I4" s="33"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+    </row>
+    <row r="5" spans="1:13" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>24</v>
+      <c r="B5" s="23" t="s">
+        <v>23</v>
       </c>
       <c r="C5" s="8">
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="11">
         <v>5</v>
@@ -968,31 +974,31 @@
         <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5" s="11">
         <v>1</v>
       </c>
-      <c r="I5" s="32">
-        <v>3</v>
-      </c>
-      <c r="J5" s="41">
-        <v>2</v>
-      </c>
-      <c r="K5" s="44">
-        <v>3</v>
-      </c>
-      <c r="L5" s="44">
+      <c r="I5" s="31">
+        <v>3</v>
+      </c>
+      <c r="J5" s="37">
+        <v>2</v>
+      </c>
+      <c r="K5" s="18">
+        <v>3</v>
+      </c>
+      <c r="L5" s="18">
         <v>4</v>
       </c>
-      <c r="M5" s="20">
+      <c r="M5" s="15">
         <f t="shared" ref="M5" si="0">-SUM(E5:E7)*$E$15-SUM(H5:H7)*$H$15+I5*$I$15+J5*$J$15+K5*$K$15+L5*$L$15</f>
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="17"/>
-      <c r="B6" s="24"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="20"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="8">
         <v>2</v>
       </c>
@@ -1002,20 +1008,20 @@
         <v>2</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="11">
         <v>3</v>
       </c>
-      <c r="I6" s="33"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-    </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="18"/>
-      <c r="B7" s="25"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+    </row>
+    <row r="7" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="2">
         <v>3</v>
       </c>
@@ -1026,24 +1032,24 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-    </row>
-    <row r="8" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I7" s="33"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+    </row>
+    <row r="8" spans="1:13" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>30</v>
+      <c r="B8" s="22" t="s">
+        <v>29</v>
       </c>
       <c r="C8" s="8">
         <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="11">
         <v>4</v>
@@ -1052,36 +1058,36 @@
         <v>1</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" s="11">
         <v>3</v>
       </c>
-      <c r="I8" s="35">
-        <v>3</v>
-      </c>
-      <c r="J8" s="41">
-        <v>3</v>
-      </c>
-      <c r="K8" s="44">
-        <v>2</v>
-      </c>
-      <c r="L8" s="44">
-        <v>3</v>
-      </c>
-      <c r="M8" s="20">
+      <c r="I8" s="34">
+        <v>3</v>
+      </c>
+      <c r="J8" s="37">
+        <v>3</v>
+      </c>
+      <c r="K8" s="18">
+        <v>2</v>
+      </c>
+      <c r="L8" s="18">
+        <v>3</v>
+      </c>
+      <c r="M8" s="15">
         <f t="shared" ref="M8" si="1">-SUM(E8:E10)*$E$15-SUM(H8:H10)*$H$15+I8*$I$15+J8*$J$15+K8*$K$15+L8*$L$15</f>
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="17"/>
-      <c r="B9" s="24"/>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="20"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="8">
         <v>2</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="11">
         <v>4</v>
@@ -1090,20 +1096,20 @@
         <v>2</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H9" s="11">
         <v>1</v>
       </c>
-      <c r="I9" s="36"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-    </row>
-    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="18"/>
-      <c r="B10" s="25"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+    </row>
+    <row r="10" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="2">
         <v>3</v>
       </c>
@@ -1114,58 +1120,78 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="13"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-    </row>
-    <row r="11" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I10" s="36"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+    </row>
+    <row r="11" spans="1:13" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="26"/>
+        <v>34</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>31</v>
+      </c>
       <c r="C11" s="8">
         <v>1</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="11"/>
+      <c r="D11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="11">
+        <v>3</v>
+      </c>
       <c r="F11" s="8">
         <v>1</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="20">
-        <f t="shared" ref="M11" si="2">-SUM(E11:E13)*E24-SUM(H11:H13)*H24+I11*I24+J11*J24+K11*K24+L11*L24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="17"/>
-      <c r="B12" s="27"/>
+      <c r="G11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="11">
+        <v>3</v>
+      </c>
+      <c r="I11" s="34">
+        <v>3</v>
+      </c>
+      <c r="J11" s="37">
+        <v>4</v>
+      </c>
+      <c r="K11" s="18">
+        <v>2</v>
+      </c>
+      <c r="L11" s="18">
+        <v>3</v>
+      </c>
+      <c r="M11" s="15">
+        <f t="shared" ref="M11" si="2">-SUM(E11:E13)*$E$15-SUM(H11:H13)*$H$15+I11*$I$15+J11*$J$15+K11*$K$15+L11*$L$15</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="20"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="8">
         <v>2</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="11"/>
       <c r="F12" s="8">
         <v>2</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-    </row>
-    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="18"/>
-      <c r="B13" s="28"/>
+      <c r="G12" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="11">
+        <v>2</v>
+      </c>
+      <c r="I12" s="35"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+    </row>
+    <row r="13" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="2">
         <v>3</v>
       </c>
@@ -1174,42 +1200,46 @@
       <c r="F13" s="2">
         <v>3</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="13">
+        <v>3</v>
+      </c>
+      <c r="I13" s="36"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="12" t="s">
+      <c r="L14" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
         <v>22</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="D15" t="s">
-        <v>23</v>
       </c>
       <c r="E15" s="12">
         <v>1</v>
@@ -1234,17 +1264,11 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="M5:M7"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="M11:M13"/>
-    <mergeCell ref="K5:K7"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="K11:K13"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="L5:L7"/>
-    <mergeCell ref="L8:L10"/>
-    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="K2:K4"/>
     <mergeCell ref="B2:B4"/>
@@ -1259,11 +1283,17 @@
     <mergeCell ref="J5:J7"/>
     <mergeCell ref="J8:J10"/>
     <mergeCell ref="J11:J13"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="M5:M7"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="M11:M13"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="L5:L7"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="L11:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>